<commit_message>
add some test sample
</commit_message>
<xml_diff>
--- a/document/测试报告.xlsx
+++ b/document/测试报告.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
   <si>
     <t>说明</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,6 +86,18 @@
   </si>
   <si>
     <t>108.275s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>40W样本中10W样本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>48684.8 s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试二</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -420,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -431,7 +443,7 @@
     <col min="1" max="9" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -439,7 +451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +459,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -455,7 +467,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -463,7 +475,7 @@
         <v>6483</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -471,7 +483,7 @@
         <v>14951</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -479,7 +491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -487,7 +499,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -495,71 +507,95 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="3">
         <v>10000</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="3">
+        <v>139181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="3">
         <v>6483</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="3">
         <v>14951</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="3">
+        <v>220487</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -567,7 +603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -575,7 +611,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -583,7 +619,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -591,7 +627,7 @@
         <v>6483</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -599,7 +635,7 @@
         <v>14951</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -607,7 +643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -615,7 +651,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -623,7 +659,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -631,7 +667,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -639,7 +675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1</v>
       </c>

</xml_diff>